<commit_message>
added testcases to flightbookTest class
</commit_message>
<xml_diff>
--- a/resource/Data.xlsx
+++ b/resource/Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -97,6 +97,12 @@
     <t xml:space="preserve">Airlines</t>
   </si>
   <si>
+    <t xml:space="preserve">Meal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Credit Card Number</t>
+  </si>
+  <si>
     <t xml:space="preserve">London</t>
   </si>
   <si>
@@ -107,6 +113,9 @@
   </si>
   <si>
     <t xml:space="preserve">Blue Skies Airlines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hindu</t>
   </si>
 </sst>
 </file>
@@ -116,7 +125,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -144,12 +153,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -194,16 +197,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -227,7 +226,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -237,7 +236,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.82"/>
@@ -335,28 +334,38 @@
       <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>122200000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>